<commit_message>
Commit - Completly finished
The document is completly finished, please proofread it
</commit_message>
<xml_diff>
--- a/Solution_Design/Story Board/Storys/RA-26 Behördenkontakte/Ra-26 Behördenkontakte_DBAufbau.xlsx
+++ b/Solution_Design/Story Board/Storys/RA-26 Behördenkontakte/Ra-26 Behördenkontakte_DBAufbau.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\GitHub\ApplicationDevelopment\Solution_Design\Story Board\Storys\RA-26 Behördenkontakte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\ApplicationDevelopment\Solution_Design\Story Board\Storys\RA-26 Behördenkontakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="0" windowWidth="18195" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Adressen" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Adressen!$A$1:$G$85</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="488">
   <si>
     <t>Straße</t>
   </si>
@@ -812,9 +813,6 @@
     <t>Carstennstraße</t>
   </si>
   <si>
-    <t>+49 (0)</t>
-  </si>
-  <si>
     <t>DRK@DRK.de</t>
   </si>
   <si>
@@ -1083,6 +1081,424 @@
   </si>
   <si>
     <t>Markplatz</t>
+  </si>
+  <si>
+    <t>Südwall</t>
+  </si>
+  <si>
+    <t>+49 (0) 2315013331</t>
+  </si>
+  <si>
+    <t>buergerdienste@stadtdo.de</t>
+  </si>
+  <si>
+    <t>buergerdienste.dortmund.de</t>
+  </si>
+  <si>
+    <t>Hollestraße</t>
+  </si>
+  <si>
+    <t>+49 (0)201 8833222</t>
+  </si>
+  <si>
+    <t>buergeramt@einwohneramt.essen.de</t>
+  </si>
+  <si>
+    <t>https://www.essen.de/rathaus/aemter/ordner_33/buergeraemter/AnmeldenVonPersonen.de.html</t>
+  </si>
+  <si>
+    <t>Stresemannstraße</t>
+  </si>
+  <si>
+    <t>+49 (0)421361-0</t>
+  </si>
+  <si>
+    <t>zentralemeldebehoerde@stadtamt.bremen.de</t>
+  </si>
+  <si>
+    <t>http://www.stadtamt.bremen.de/sixcms/detail.php?gsid=bremen116.c.1626.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Am Augustinerhof </t>
+  </si>
+  <si>
+    <t>+49 (0)651718-0</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>http://www.trier.de/Rathaus-Buerger-in/Stadtverwaltung/Aemter-Dienststellen/Dezernat-III/Buergeramt/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theaterstraße </t>
+  </si>
+  <si>
+    <t>+49 (0)351 488-6070</t>
+  </si>
+  <si>
+    <t>buergerbuero-altstadt@dresden.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berliner Platz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+49 (0)641 306-1234
+</t>
+  </si>
+  <si>
+    <t>stadtbuero@giessen.de</t>
+  </si>
+  <si>
+    <t>https://www.giessen.de/Rathaus_und_Service/B%C3%BCrgerservice/Stadtb%C3%BCro/Erstwohnsitz/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liebertwolkwitzer Markt </t>
+  </si>
+  <si>
+    <t>buergeramt@leipzig.de</t>
+  </si>
+  <si>
+    <t>'+49(0)341123-0</t>
+  </si>
+  <si>
+    <t>http://www.berlin.de/ba-mitte/politik-und-verwaltung/aemter/amt-fuer-soziales/</t>
+  </si>
+  <si>
+    <t>nach Vereinabrung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beusselstraße </t>
+  </si>
+  <si>
+    <t>44 n-q </t>
+  </si>
+  <si>
+    <t>welcome@berliner-tafel.de </t>
+  </si>
+  <si>
+    <t>www.berliner-tafel.de</t>
+  </si>
+  <si>
+    <t>Thalkirchner Straße  </t>
+  </si>
+  <si>
+    <t>www.muenchner-tafel.de</t>
+  </si>
+  <si>
+    <t>info@muenchner-tafel.de </t>
+  </si>
+  <si>
+    <t>info@hamburger-tafel.de </t>
+  </si>
+  <si>
+    <t>www.hamburger-tafel.de</t>
+  </si>
+  <si>
+    <t>+49 (0)30 115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+49 (0)30 7827414 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)40 443646 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)89 292250 </t>
+  </si>
+  <si>
+    <t>Bramfelder Straße </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirschbaumweg </t>
+  </si>
+  <si>
+    <t>18 A </t>
+  </si>
+  <si>
+    <t>14 b</t>
+  </si>
+  <si>
+    <t>Riederhofstraße</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brückenstraße </t>
+  </si>
+  <si>
+    <t>mail@stuttgarter-tafel.de </t>
+  </si>
+  <si>
+    <t>www.schwaebische-tafel-stuttgart.de</t>
+  </si>
+  <si>
+    <t>Völklinger Straße</t>
+  </si>
+  <si>
+    <t>31-35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osterlandwehr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Steeler Straße </t>
+  </si>
+  <si>
+    <t>137 </t>
+  </si>
+  <si>
+    <t>Brauerstraße</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>Jordanstraße</t>
+  </si>
+  <si>
+    <t>Krahnenstraße</t>
+  </si>
+  <si>
+    <t>1 Zwickauer Straße</t>
+  </si>
+  <si>
+    <t>01069 </t>
+  </si>
+  <si>
+    <t>Gartenstraße 11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)641 9322836 </t>
+  </si>
+  <si>
+    <t>'+49 (0)711 6338990</t>
+  </si>
+  <si>
+    <t>giessener.tafel@diakonie-giessen.de </t>
+  </si>
+  <si>
+    <t>www.giessener-tafel.de </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)351 4481210 </t>
+  </si>
+  <si>
+    <t> info@dresdner-tafel.de </t>
+  </si>
+  <si>
+    <t>www.dresdner-tafel.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)651 9496171 </t>
+  </si>
+  <si>
+    <t>h.neumaerker@skf-trier.de </t>
+  </si>
+  <si>
+    <t> www.skf-trier.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)341 68 98 481 </t>
+  </si>
+  <si>
+    <t>kontakt@leipziger-tafel.de </t>
+  </si>
+  <si>
+    <t> www.leipziger-tafel.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)421 4341959 </t>
+  </si>
+  <si>
+    <t>brementafel@nord-com.net </t>
+  </si>
+  <si>
+    <t> www.bremertafel.de </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)201 2720255 </t>
+  </si>
+  <si>
+    <t>essener_tafel@gmx.de </t>
+  </si>
+  <si>
+    <t> www.essener-tafel.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)231 4773240 </t>
+  </si>
+  <si>
+    <t>info@dortmunder-tafel.de </t>
+  </si>
+  <si>
+    <t>www.dortmunder-tafel.de</t>
+  </si>
+  <si>
+    <t>'+49 (0)211 43 60 103</t>
+  </si>
+  <si>
+    <t>info@duesseldorfer-tafel.de</t>
+  </si>
+  <si>
+    <t>www.duesseldorfer-tafel.de</t>
+  </si>
+  <si>
+    <t> frankfurtertafel@t-online.de </t>
+  </si>
+  <si>
+    <t>www.frankfurter-tafel.de</t>
+  </si>
+  <si>
+    <t>info@koelner-tafel.de </t>
+  </si>
+  <si>
+    <t> www.koelner-tafel.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)221351000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'+49 (0)69 4980825 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurt-Schumacher-Allee </t>
+  </si>
+  <si>
+    <t>Schwanthalerstraße</t>
+  </si>
+  <si>
+    <t>Eschersheimer Landstraße</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willi-Becker-Allee </t>
+  </si>
+  <si>
+    <t>+49 (0)211 8991</t>
+  </si>
+  <si>
+    <t>+49 (0)711 21659000</t>
+  </si>
+  <si>
+    <t>soziale-sicherung@stadt.duesseldorf.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplerbecker Marktplatz </t>
+  </si>
+  <si>
+    <t>+49 (0)23150 29 349</t>
+  </si>
+  <si>
+    <t>sozialamt@dortmund.de</t>
+  </si>
+  <si>
+    <t>http://www.dortmund.de/de/leben_in_dortmund/familie_und_soziales/sozialamt/start_sozialamt/index.html</t>
+  </si>
+  <si>
+    <t>http://www.muenchen.de/rathaus/Stadtverwaltung/Sozialreferat/Sozialamt.html</t>
+  </si>
+  <si>
+    <t>https://www.hamburg.de/behoerdenfinder/hamburg/info/sozialamt/</t>
+  </si>
+  <si>
+    <t>bezirksamt@hamburg-mitte.hamburg.de</t>
+  </si>
+  <si>
+    <t>+49 (0)40428544591</t>
+  </si>
+  <si>
+    <t>+49 (0)8923396805</t>
+  </si>
+  <si>
+    <t>sbh-mitte.soz@muenchen.de</t>
+  </si>
+  <si>
+    <t>+49 (0)2212210</t>
+  </si>
+  <si>
+    <t>sozialamt@stadt-koeln.de</t>
+  </si>
+  <si>
+    <t>Werktage ohne Mi</t>
+  </si>
+  <si>
+    <t>http://www.stadt-koeln.de/service/adressen/amt-fuer-soziales-und-senioren-aussenstelle-innenstadt</t>
+  </si>
+  <si>
+    <t>+49 (0)69212-449-00</t>
+  </si>
+  <si>
+    <t>http://www.frankfurt.de/sixcms/detail.php?id=2983</t>
+  </si>
+  <si>
+    <t>https://www.stuttgart.de/item/show/305802/1/dept/4567?</t>
+  </si>
+  <si>
+    <t>http://www.use24.essen.de/Webportal/agency/default.aspx?OrganizationUnitId=257</t>
+  </si>
+  <si>
+    <t>sozialamt@essen.de</t>
+  </si>
+  <si>
+    <t>+49 (0)201 88 50001</t>
+  </si>
+  <si>
+    <t>Steubenstraße</t>
+  </si>
+  <si>
+    <t>http://www.amtfuersozialedienste.bremen.de/sixcms/detail.php?gsid=bremen02.c.730.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hans-Böckler-Straße </t>
+  </si>
+  <si>
+    <t>office@afsd.bremen.de</t>
+  </si>
+  <si>
+    <t>+49 (0)421 361-8295</t>
+  </si>
+  <si>
+    <t>http://www.leipzig.de/buergerservice-und-verwaltung/aemter-und-behoerdengaenge/behoerden-und-dienstleistungen/dienststelle/sozialamt-50/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burgplatz </t>
+  </si>
+  <si>
+    <t>+49 (0)341123-4521</t>
+  </si>
+  <si>
+    <t>sozialamt@leipzig.de</t>
+  </si>
+  <si>
+    <t>Am Augustinerhof</t>
+  </si>
+  <si>
+    <t>Rathaus Verwaltungsgebäude II</t>
+  </si>
+  <si>
+    <t>+49 (0)651 / 718-150-9</t>
+  </si>
+  <si>
+    <t>http://www.dresden.de/de/rathaus/aemter-und-einrichtungen/oe/dborg/stadt_dresden_6503.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junghansstraße </t>
+  </si>
+  <si>
+    <t>+49 (0)351/ 488-4831</t>
+  </si>
+  <si>
+    <t>sozialleistungen@dresden.de</t>
+  </si>
+  <si>
+    <t>+49 (0)351/ 488-4830</t>
+  </si>
+  <si>
+    <t>sozialamt@lkgi.de</t>
+  </si>
+  <si>
+    <t>+49 (0)641 / 9390-0</t>
+  </si>
+  <si>
+    <t>Sozialamt Gießen Der Kreisauschuss</t>
   </si>
 </sst>
 </file>
@@ -1091,9 +1507,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00000"/>
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1123,6 +1539,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF003165"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1145,7 +1580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1185,9 +1620,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1207,9 +1648,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1247,7 +1688,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1319,7 +1760,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1470,12 +1911,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H64" sqref="H62:H64"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,16 +1936,16 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -2789,7 +3230,7 @@
         <v>56</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E57" s="6">
         <v>146</v>
@@ -2812,7 +3253,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E58" s="6">
         <v>47</v>
@@ -2835,7 +3276,7 @@
         <v>58</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E59" s="6">
         <v>11</v>
@@ -2858,7 +3299,7 @@
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E60" s="6">
         <v>1</v>
@@ -2881,10 +3322,10 @@
         <v>60</v>
       </c>
       <c r="D61" t="s">
+        <v>333</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>334</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>335</v>
       </c>
       <c r="F61" s="3">
         <v>60320</v>
@@ -2927,7 +3368,7 @@
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E63" s="6">
         <v>33</v>
@@ -2950,7 +3391,7 @@
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E64" s="6">
         <v>2</v>
@@ -2972,7 +3413,15 @@
       <c r="C65" s="2">
         <v>64</v>
       </c>
-      <c r="F65" s="3"/>
+      <c r="D65" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E65" s="6">
+        <v>2</v>
+      </c>
+      <c r="F65" s="3">
+        <v>44137</v>
+      </c>
       <c r="G65" s="2" t="s">
         <v>202</v>
       </c>
@@ -2987,7 +3436,15 @@
       <c r="C66" s="2">
         <v>65</v>
       </c>
-      <c r="F66" s="3"/>
+      <c r="D66" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E66" s="6">
+        <v>3</v>
+      </c>
+      <c r="F66" s="3">
+        <v>45127</v>
+      </c>
       <c r="G66" s="2" t="s">
         <v>78</v>
       </c>
@@ -3002,7 +3459,15 @@
       <c r="C67" s="2">
         <v>66</v>
       </c>
-      <c r="F67" s="3"/>
+      <c r="D67" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E67" s="6">
+        <v>48</v>
+      </c>
+      <c r="F67" s="3">
+        <v>28207</v>
+      </c>
       <c r="G67" s="2" t="s">
         <v>47</v>
       </c>
@@ -3017,7 +3482,15 @@
       <c r="C68" s="2">
         <v>67</v>
       </c>
-      <c r="F68" s="3"/>
+      <c r="D68" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="E68" s="6">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3">
+        <v>4288</v>
+      </c>
       <c r="G68" s="2" t="s">
         <v>102</v>
       </c>
@@ -3032,7 +3505,15 @@
       <c r="C69" s="2">
         <v>68</v>
       </c>
-      <c r="F69" s="3"/>
+      <c r="D69" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="E69" s="6">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3">
+        <v>54290</v>
+      </c>
       <c r="G69" s="2" t="s">
         <v>203</v>
       </c>
@@ -3047,7 +3528,15 @@
       <c r="C70" s="2">
         <v>69</v>
       </c>
-      <c r="F70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E70" s="6">
+        <v>11</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1067</v>
+      </c>
       <c r="G70" s="2" t="s">
         <v>204</v>
       </c>
@@ -3062,7 +3551,15 @@
       <c r="C71" s="2">
         <v>70</v>
       </c>
-      <c r="F71" s="3"/>
+      <c r="D71" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E71" s="6">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3">
+        <v>35390</v>
+      </c>
       <c r="G71" s="2" t="s">
         <v>205</v>
       </c>
@@ -3077,7 +3574,15 @@
       <c r="C72" s="2">
         <v>71</v>
       </c>
-      <c r="F72" s="3"/>
+      <c r="D72" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E72" s="6">
+        <v>146</v>
+      </c>
+      <c r="F72" s="3">
+        <v>13353</v>
+      </c>
       <c r="G72" s="2" t="s">
         <v>43</v>
       </c>
@@ -3092,7 +3597,15 @@
       <c r="C73" s="2">
         <v>72</v>
       </c>
-      <c r="F73" s="3"/>
+      <c r="D73" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E73" s="2">
+        <v>4</v>
+      </c>
+      <c r="F73" s="3">
+        <v>20095</v>
+      </c>
       <c r="G73" s="2" t="s">
         <v>55</v>
       </c>
@@ -3107,7 +3620,15 @@
       <c r="C74" s="2">
         <v>73</v>
       </c>
-      <c r="F74" s="3"/>
+      <c r="D74" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E74" s="6">
+        <v>62</v>
+      </c>
+      <c r="F74" s="3">
+        <v>80336</v>
+      </c>
       <c r="G74" s="2" t="s">
         <v>91</v>
       </c>
@@ -3122,7 +3643,15 @@
       <c r="C75" s="2">
         <v>74</v>
       </c>
-      <c r="F75" s="3"/>
+      <c r="D75" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E75" s="6">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3">
+        <v>51103</v>
+      </c>
       <c r="G75" s="2" t="s">
         <v>201</v>
       </c>
@@ -3137,7 +3666,15 @@
       <c r="C76" s="2">
         <v>75</v>
       </c>
-      <c r="F76" s="3"/>
+      <c r="D76" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F76" s="3">
+        <v>60320</v>
+      </c>
       <c r="G76" s="2" t="s">
         <v>63</v>
       </c>
@@ -3152,7 +3689,15 @@
       <c r="C77" s="2">
         <v>76</v>
       </c>
-      <c r="F77" s="3"/>
+      <c r="D77" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E77" s="6">
+        <v>33</v>
+      </c>
+      <c r="F77" s="3">
+        <v>70713</v>
+      </c>
       <c r="G77" s="2" t="s">
         <v>126</v>
       </c>
@@ -3167,7 +3712,15 @@
       <c r="C78" s="2">
         <v>77</v>
       </c>
-      <c r="F78" s="3"/>
+      <c r="D78" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E78" s="6">
+        <v>8</v>
+      </c>
+      <c r="F78" s="3">
+        <v>40200</v>
+      </c>
       <c r="G78" s="2" t="s">
         <v>108</v>
       </c>
@@ -3182,7 +3735,15 @@
       <c r="C79" s="2">
         <v>78</v>
       </c>
-      <c r="F79" s="3"/>
+      <c r="D79" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E79" s="6">
+        <v>21</v>
+      </c>
+      <c r="F79" s="3">
+        <v>44287</v>
+      </c>
       <c r="G79" s="2" t="s">
         <v>202</v>
       </c>
@@ -3197,12 +3758,20 @@
       <c r="C80" s="2">
         <v>79</v>
       </c>
-      <c r="F80" s="3"/>
+      <c r="D80" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="E80" s="6">
+        <v>53</v>
+      </c>
+      <c r="F80" s="3">
+        <v>45138</v>
+      </c>
       <c r="G80" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>3</v>
       </c>
@@ -3212,12 +3781,21 @@
       <c r="C81" s="2">
         <v>80</v>
       </c>
-      <c r="F81" s="3"/>
+      <c r="D81" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="E81" s="6">
+        <v>9</v>
+      </c>
+      <c r="F81" s="3">
+        <v>28217</v>
+      </c>
       <c r="G81" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J81" s="19"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>3</v>
       </c>
@@ -3227,12 +3805,21 @@
       <c r="C82" s="2">
         <v>81</v>
       </c>
-      <c r="F82" s="3"/>
+      <c r="D82" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E82" s="6">
+        <v>1</v>
+      </c>
+      <c r="F82" s="3">
+        <v>4092</v>
+      </c>
       <c r="G82" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J82" s="19"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>3</v>
       </c>
@@ -3242,12 +3829,20 @@
       <c r="C83" s="2">
         <v>82</v>
       </c>
-      <c r="F83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="F83" s="3">
+        <v>54290</v>
+      </c>
       <c r="G83" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>3</v>
       </c>
@@ -3257,12 +3852,20 @@
       <c r="C84" s="2">
         <v>83</v>
       </c>
-      <c r="F84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="E84" s="6">
+        <v>2</v>
+      </c>
+      <c r="F84" s="3">
+        <v>1277</v>
+      </c>
       <c r="G84" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>3</v>
       </c>
@@ -3272,12 +3875,20 @@
       <c r="C85" s="2">
         <v>84</v>
       </c>
-      <c r="F85" s="3"/>
+      <c r="D85" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="F85" s="3">
+        <v>35394</v>
+      </c>
       <c r="G85" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>4</v>
       </c>
@@ -3287,7 +3898,7 @@
       <c r="C86" s="2">
         <v>85</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="3" t="s">
         <v>244</v>
       </c>
       <c r="E86" s="6">
@@ -3300,7 +3911,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>9</v>
       </c>
@@ -3323,7 +3934,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>9</v>
       </c>
@@ -3346,7 +3957,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>7</v>
       </c>
@@ -3369,7 +3980,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>7</v>
       </c>
@@ -3392,7 +4003,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>7</v>
       </c>
@@ -3403,7 +4014,7 @@
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E91" s="6">
         <v>5</v>
@@ -3412,10 +4023,10 @@
         <v>14469</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>7</v>
       </c>
@@ -3426,7 +4037,7 @@
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E92" s="6">
         <v>11</v>
@@ -3438,7 +4049,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>7</v>
       </c>
@@ -3449,19 +4060,19 @@
         <v>92</v>
       </c>
       <c r="D93" t="s">
+        <v>268</v>
+      </c>
+      <c r="E93" t="s">
         <v>269</v>
-      </c>
-      <c r="E93" t="s">
-        <v>270</v>
       </c>
       <c r="F93" s="2">
         <v>79110</v>
       </c>
       <c r="G93" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>7</v>
       </c>
@@ -3472,7 +4083,7 @@
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E94" s="6">
         <v>90</v>
@@ -3484,7 +4095,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>7</v>
       </c>
@@ -3495,7 +4106,7 @@
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E95" s="6">
         <v>25</v>
@@ -3504,11 +4115,330 @@
         <v>54329</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D96"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>8</v>
+      </c>
+      <c r="B96" s="2">
+        <v>6</v>
+      </c>
+      <c r="C96" s="2">
+        <v>95</v>
+      </c>
+      <c r="D96" t="s">
+        <v>377</v>
+      </c>
+      <c r="E96" t="s">
+        <v>378</v>
+      </c>
+      <c r="F96" s="2">
+        <v>10553</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>8</v>
+      </c>
+      <c r="B97" s="2">
+        <v>6</v>
+      </c>
+      <c r="C97" s="2">
+        <v>96</v>
+      </c>
+      <c r="D97" t="s">
+        <v>390</v>
+      </c>
+      <c r="E97" s="14">
+        <v>102</v>
+      </c>
+      <c r="F97" s="2">
+        <v>22305</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>8</v>
+      </c>
+      <c r="B98" s="2">
+        <v>6</v>
+      </c>
+      <c r="C98" s="2">
+        <v>97</v>
+      </c>
+      <c r="D98" t="s">
+        <v>381</v>
+      </c>
+      <c r="E98" s="6">
+        <v>81</v>
+      </c>
+      <c r="F98" s="2">
+        <v>81371</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>8</v>
+      </c>
+      <c r="B99" s="2">
+        <v>6</v>
+      </c>
+      <c r="C99" s="2">
+        <v>98</v>
+      </c>
+      <c r="D99" t="s">
+        <v>391</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="F99" s="2">
+        <v>50996</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>8</v>
+      </c>
+      <c r="B100" s="2">
+        <v>6</v>
+      </c>
+      <c r="C100" s="2">
+        <v>99</v>
+      </c>
+      <c r="D100" t="s">
+        <v>394</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="F100" s="2">
+        <v>60314</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>8</v>
+      </c>
+      <c r="B101" s="2">
+        <v>6</v>
+      </c>
+      <c r="C101" s="2">
+        <v>100</v>
+      </c>
+      <c r="D101" t="s">
+        <v>395</v>
+      </c>
+      <c r="E101" s="6">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2">
+        <v>70376</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>8</v>
+      </c>
+      <c r="B102" s="2">
+        <v>6</v>
+      </c>
+      <c r="C102" s="2">
+        <v>101</v>
+      </c>
+      <c r="D102" t="s">
+        <v>398</v>
+      </c>
+      <c r="E102" s="6">
+        <v>24</v>
+      </c>
+      <c r="F102" s="2">
+        <v>40221</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>8</v>
+      </c>
+      <c r="B103" s="2">
+        <v>6</v>
+      </c>
+      <c r="C103" s="2">
+        <v>102</v>
+      </c>
+      <c r="D103" t="s">
+        <v>400</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="F103" s="2">
+        <v>44145</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>8</v>
+      </c>
+      <c r="B104" s="2">
+        <v>6</v>
+      </c>
+      <c r="C104" s="2">
+        <v>103</v>
+      </c>
+      <c r="D104" t="s">
+        <v>401</v>
+      </c>
+      <c r="E104" t="s">
+        <v>402</v>
+      </c>
+      <c r="F104" s="2">
+        <v>45138</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>8</v>
+      </c>
+      <c r="B105" s="2">
+        <v>6</v>
+      </c>
+      <c r="C105" s="2">
+        <v>104</v>
+      </c>
+      <c r="D105" t="s">
+        <v>403</v>
+      </c>
+      <c r="E105" s="14">
+        <v>13</v>
+      </c>
+      <c r="F105" s="2">
+        <v>28309</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>8</v>
+      </c>
+      <c r="B106" s="2">
+        <v>6</v>
+      </c>
+      <c r="C106" s="2">
+        <v>105</v>
+      </c>
+      <c r="D106" t="s">
+        <v>405</v>
+      </c>
+      <c r="E106" t="s">
+        <v>404</v>
+      </c>
+      <c r="F106" s="3">
+        <v>4177</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>8</v>
+      </c>
+      <c r="B107" s="2">
+        <v>6</v>
+      </c>
+      <c r="C107" s="2">
+        <v>106</v>
+      </c>
+      <c r="D107" t="s">
+        <v>406</v>
+      </c>
+      <c r="E107" s="14">
+        <v>35</v>
+      </c>
+      <c r="F107" s="2">
+        <v>54290</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>8</v>
+      </c>
+      <c r="B108" s="2">
+        <v>6</v>
+      </c>
+      <c r="C108" s="2">
+        <v>107</v>
+      </c>
+      <c r="D108" t="s">
+        <v>407</v>
+      </c>
+      <c r="E108" s="6">
+        <v>32</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>8</v>
+      </c>
+      <c r="B109" s="2">
+        <v>6</v>
+      </c>
+      <c r="C109" s="2">
+        <v>108</v>
+      </c>
+      <c r="D109" t="s">
+        <v>409</v>
+      </c>
+      <c r="E109" s="6">
+        <v>11</v>
+      </c>
+      <c r="F109" s="2">
+        <v>35390</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G85"/>
@@ -3520,10 +4450,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="G137" sqref="G137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3540,19 +4470,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>308</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>309</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>4</v>
@@ -5014,7 +5944,7 @@
         <v>56</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C66" s="7">
         <v>5</v>
@@ -5026,10 +5956,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="F66" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -5037,7 +5967,7 @@
         <v>56</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C67" s="7">
         <v>7</v>
@@ -5049,10 +5979,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="F67" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -5060,7 +5990,7 @@
         <v>57</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C68" s="7">
         <v>2</v>
@@ -5072,10 +6002,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="F68" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -5083,7 +6013,7 @@
         <v>58</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C69" s="7">
         <v>3</v>
@@ -5095,10 +6025,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -5106,7 +6036,7 @@
         <v>58</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C70" s="7">
         <v>7</v>
@@ -5118,10 +6048,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -5129,7 +6059,7 @@
         <v>58</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C71" s="7">
         <v>8</v>
@@ -5141,10 +6071,10 @@
         <v>0.5625</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -5152,7 +6082,7 @@
         <v>59</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C72" s="7">
         <v>4</v>
@@ -5167,7 +6097,7 @@
         <v>210</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -5175,7 +6105,7 @@
         <v>59</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C73" s="7">
         <v>5</v>
@@ -5190,7 +6120,7 @@
         <v>210</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -5198,7 +6128,7 @@
         <v>59</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C74" s="7">
         <v>7</v>
@@ -5213,7 +6143,7 @@
         <v>210</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -5221,7 +6151,7 @@
         <v>59</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C75" s="7">
         <v>8</v>
@@ -5236,7 +6166,7 @@
         <v>210</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -5244,7 +6174,7 @@
         <v>60</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C76" s="7">
         <v>2</v>
@@ -5256,10 +6186,10 @@
         <v>0.75</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -5267,7 +6197,7 @@
         <v>61</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C77" s="7">
         <v>2</v>
@@ -5290,7 +6220,7 @@
         <v>62</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C78" s="7">
         <v>0</v>
@@ -5302,10 +6232,10 @@
         <v>210</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -5313,7 +6243,7 @@
         <v>63</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C79" s="7">
         <v>0</v>
@@ -5325,10 +6255,10 @@
         <v>210</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -5336,403 +6266,1909 @@
         <v>64</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C80" s="7"/>
+        <v>350</v>
+      </c>
+      <c r="C80" s="7">
+        <v>4</v>
+      </c>
+      <c r="D80" s="15">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E80" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C81" s="7"/>
+        <v>350</v>
+      </c>
+      <c r="C81" s="7">
+        <v>5</v>
+      </c>
+      <c r="D81" s="15">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E81" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C82" s="7"/>
+        <v>350</v>
+      </c>
+      <c r="C82" s="7">
+        <v>7</v>
+      </c>
+      <c r="D82" s="15">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E82" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C83" s="7"/>
+        <v>350</v>
+      </c>
+      <c r="C83" s="7">
+        <v>8</v>
+      </c>
+      <c r="D83" s="15">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E83" s="15">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C84" s="7"/>
+        <v>354</v>
+      </c>
+      <c r="C84" s="7">
+        <v>4</v>
+      </c>
+      <c r="D84" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E84" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F84" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C85" s="7"/>
+        <v>354</v>
+      </c>
+      <c r="C85" s="7">
+        <v>5</v>
+      </c>
+      <c r="D85" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E85" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F85" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C86" s="7"/>
+        <v>354</v>
+      </c>
+      <c r="C86" s="7">
+        <v>6</v>
+      </c>
+      <c r="D86" s="15">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E86" s="15">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F86" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C87" s="7"/>
+        <v>354</v>
+      </c>
+      <c r="C87" s="7">
+        <v>7</v>
+      </c>
+      <c r="D87" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E87" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F87" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C88" s="7"/>
+        <v>354</v>
+      </c>
+      <c r="C88" s="7">
+        <v>8</v>
+      </c>
+      <c r="D88" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E88" s="15">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F88" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C89" s="7"/>
+        <v>358</v>
+      </c>
+      <c r="C89" s="7">
+        <v>1</v>
+      </c>
+      <c r="D89" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E89" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C90" s="7"/>
+        <v>374</v>
+      </c>
+      <c r="C90" s="7">
+        <v>5</v>
+      </c>
+      <c r="D90" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E90" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C91" s="7"/>
+        <v>374</v>
+      </c>
+      <c r="C91" s="7">
+        <v>6</v>
+      </c>
+      <c r="D91" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E91" s="15">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C92" s="7"/>
+        <v>374</v>
+      </c>
+      <c r="C92" s="7">
+        <v>7</v>
+      </c>
+      <c r="D92" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E92" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C93" s="7"/>
+        <v>374</v>
+      </c>
+      <c r="C93" s="7">
+        <v>8</v>
+      </c>
+      <c r="D93" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E93" s="15">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>274</v>
+        <v>362</v>
       </c>
       <c r="C94" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D94" s="15">
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E94" s="15">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>245</v>
+        <v>0.75</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>363</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>246</v>
+        <v>364</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>259</v>
+        <v>362</v>
       </c>
       <c r="C95" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D95" s="15">
-        <v>0.35416666666666669</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="E95" s="15">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G95" s="10" t="s">
-        <v>250</v>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>259</v>
+        <v>362</v>
       </c>
       <c r="C96" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D96" s="15">
-        <v>0.35416666666666669</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="E96" s="15">
-        <v>0.72916666666666663</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>250</v>
+        <v>363</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>259</v>
+        <v>362</v>
       </c>
       <c r="C97" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D97" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E97" s="15">
         <v>0.75</v>
       </c>
-      <c r="E97" s="15">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>261</v>
+      <c r="F97" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>286</v>
+        <v>362</v>
       </c>
       <c r="C98" s="7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D98" s="15">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E98" s="15">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>254</v>
+        <v>0.625</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>259</v>
+        <v>366</v>
       </c>
       <c r="C99" s="7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D99" s="15">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E99" s="15">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>264</v>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="G99" s="9" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>272</v>
+        <v>366</v>
       </c>
       <c r="C100" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D100" s="15">
         <v>0.33333333333333331</v>
       </c>
       <c r="E100" s="15">
-        <v>0.625</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>267</v>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F100" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>272</v>
+        <v>366</v>
       </c>
       <c r="C101" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D101" s="15">
         <v>0.33333333333333331</v>
       </c>
       <c r="E101" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>267</v>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="G101" s="9" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>273</v>
+        <v>366</v>
       </c>
       <c r="C102" s="7">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D102" s="15">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E102" s="15">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>276</v>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>279</v>
+        <v>366</v>
       </c>
       <c r="C103" s="7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D103" s="15">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E103" s="15">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>280</v>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F103" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
+        <v>69</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C104" s="7">
+        <v>9</v>
+      </c>
+      <c r="D104" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E104" s="15">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F104" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="G104" s="9" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>70</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C105" s="7">
+        <v>4</v>
+      </c>
+      <c r="D105" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E105" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G105" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>70</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C106" s="7">
+        <v>5</v>
+      </c>
+      <c r="D106" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E106" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>70</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C107" s="7">
+        <v>6</v>
+      </c>
+      <c r="D107" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E107" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>70</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C108" s="7">
+        <v>7</v>
+      </c>
+      <c r="D108" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E108" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>70</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C109" s="7">
+        <v>8</v>
+      </c>
+      <c r="D109" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E109" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G109" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>70</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C110" s="7">
+        <v>9</v>
+      </c>
+      <c r="D110" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E110" s="15">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G110" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>71</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C111" s="7">
+        <v>13</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="G111" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>72</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="C112" s="7">
+        <v>4</v>
+      </c>
+      <c r="D112" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E112" s="15">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>72</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="C113" s="7">
+        <v>7</v>
+      </c>
+      <c r="D113" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E113" s="15">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>73</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C114" s="7">
+        <v>4</v>
+      </c>
+      <c r="D114" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E114" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F114" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>73</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C115" s="7">
+        <v>5</v>
+      </c>
+      <c r="D115" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E115" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F115" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>73</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C116" s="7">
+        <v>6</v>
+      </c>
+      <c r="D116" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E116" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F116" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>73</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C117" s="7">
+        <v>7</v>
+      </c>
+      <c r="D117" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E117" s="15">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>73</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C118" s="7">
+        <v>8</v>
+      </c>
+      <c r="D118" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E118" s="15">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>74</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C119" s="7">
+        <v>14</v>
+      </c>
+      <c r="D119" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E119" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F119" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="G119" s="9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>75</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="C120" s="7">
+        <v>13</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E120" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="F120" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="G120" s="9" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>76</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="G121" s="9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>77</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="C122" s="7">
+        <v>4</v>
+      </c>
+      <c r="D122" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E122" s="15">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="G122" s="9" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>78</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="C123" s="7">
+        <v>4</v>
+      </c>
+      <c r="D123" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E123" s="15">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F123" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="G123" s="9" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>78</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="C124" s="7">
+        <v>7</v>
+      </c>
+      <c r="D124" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E124" s="15">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F124" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="G124" s="9" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>79</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="C125" s="7">
+        <v>1</v>
+      </c>
+      <c r="D125" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E125" s="15">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F125" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="G125" s="9" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>80</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C126" s="7">
+        <v>4</v>
+      </c>
+      <c r="D126" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E126" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F126" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="G126" s="9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>81</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C127" s="7">
+        <v>5</v>
+      </c>
+      <c r="D127" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E127" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="G127" s="9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>82</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C128" s="7">
+        <v>6</v>
+      </c>
+      <c r="D128" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E128" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="G128" s="9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>83</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C129" s="7">
+        <v>7</v>
+      </c>
+      <c r="D129" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E129" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F129" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="G129" s="9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>84</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="C130" s="7">
+        <v>8</v>
+      </c>
+      <c r="D130" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E130" s="15">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="G130" s="9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>81</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C131" s="7">
+        <v>1</v>
+      </c>
+      <c r="D131" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E131" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F131" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="G131" s="9" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>82</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="C132" s="7">
+        <v>4</v>
+      </c>
+      <c r="D132" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E132" s="15">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F132" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G132" s="9" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>82</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="C133" s="7">
+        <v>6</v>
+      </c>
+      <c r="D133" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E133" s="15">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F133" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G133" s="9" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>82</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="C134" s="7">
+        <v>8</v>
+      </c>
+      <c r="D134" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E134" s="15">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F134" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G134" s="9" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>83</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="C135" s="7">
+        <v>5</v>
+      </c>
+      <c r="D135" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E135" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F135" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="G135" s="9" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>83</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C136" s="7">
+        <v>7</v>
+      </c>
+      <c r="D136" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E136" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F136" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="G136" s="9" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>84</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="C137" s="7">
+        <v>13</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E137" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F137" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="G137" s="17" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>85</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C138" s="7">
+        <v>2</v>
+      </c>
+      <c r="D138" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E138" s="15">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F138" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G138" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>86</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C139" s="7">
+        <v>2</v>
+      </c>
+      <c r="D139" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E139" s="15">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G139" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
         <v>87</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B140" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C140" s="7">
+        <v>2</v>
+      </c>
+      <c r="D140" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E140" s="15">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F140" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G140" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>88</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C141" s="7">
+        <v>1</v>
+      </c>
+      <c r="D141" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="E141" s="15">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G141" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>89</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C142" s="7">
+        <v>12</v>
+      </c>
+      <c r="D142" s="15">
+        <v>0</v>
+      </c>
+      <c r="E142" s="15">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G142" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>90</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C143" s="7">
+        <v>12</v>
+      </c>
+      <c r="D143" s="15">
+        <v>0</v>
+      </c>
+      <c r="E143" s="15">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>91</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C144" s="7">
+        <v>3</v>
+      </c>
+      <c r="D144" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E144" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>92</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C145" s="7">
+        <v>8</v>
+      </c>
+      <c r="D145" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E145" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>93</v>
+      </c>
+      <c r="B146" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C146" s="7">
+        <v>12</v>
+      </c>
+      <c r="D146" s="15">
+        <v>0</v>
+      </c>
+      <c r="E146" s="15">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>94</v>
+      </c>
+      <c r="B147" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C147" s="7">
+        <v>12</v>
+      </c>
+      <c r="D147" s="15">
+        <v>0</v>
+      </c>
+      <c r="E147" s="15">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>95</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C148" s="7">
+        <v>12</v>
+      </c>
+      <c r="D148" s="15">
+        <v>0</v>
+      </c>
+      <c r="E148" s="15">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="F148" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C104" s="7">
-        <v>12</v>
-      </c>
-      <c r="D104" s="15">
-        <v>0</v>
-      </c>
-      <c r="E104" s="15">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="F104" s="1" t="s">
+      <c r="G148" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="G104" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="8"/>
-      <c r="C105" s="7"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="8"/>
-      <c r="C106" s="7"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="8"/>
-      <c r="C107" s="7"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="8"/>
-      <c r="C108" s="7"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="8"/>
-      <c r="C109" s="7"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="8"/>
-      <c r="C110" s="7"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>95</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D149" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E149" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>96</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E150" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>97</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D151" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E151" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>98</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D152" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E152" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>99</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D153" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E153" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>100</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D154" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E154" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>101</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D155" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E155" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>102</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D156" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E156" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>103</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D157" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E157" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>104</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D158" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E158" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>105</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D159" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E159" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G159" s="18" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>106</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D160" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E160" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>107</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C161" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D161" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E161" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>108</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D162" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="E162" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>413</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5772,23 +8208,23 @@
     <hyperlink ref="F47" r:id="rId34"/>
     <hyperlink ref="F48" r:id="rId35"/>
     <hyperlink ref="F49" r:id="rId36"/>
-    <hyperlink ref="G95" r:id="rId37"/>
-    <hyperlink ref="F95" r:id="rId38" display="mailto:office@berlin.msf.org"/>
-    <hyperlink ref="G96" r:id="rId39"/>
-    <hyperlink ref="F97" r:id="rId40" display="mailto:info@drk-westfalen.de"/>
-    <hyperlink ref="F98" r:id="rId41"/>
-    <hyperlink ref="G98" r:id="rId42"/>
-    <hyperlink ref="G97" r:id="rId43"/>
-    <hyperlink ref="G99" r:id="rId44"/>
-    <hyperlink ref="F99" r:id="rId45" display="mailto:info@drk-lv-brandenburg.de"/>
-    <hyperlink ref="G101" r:id="rId46" display="http://www.drk-berlin.de/"/>
-    <hyperlink ref="F101" r:id="rId47" display="mailto:drk@drk-berlin.de"/>
-    <hyperlink ref="F102" r:id="rId48" display="http://www.drk-baden.de/"/>
-    <hyperlink ref="G102" r:id="rId49" display="mailto:pressestelle@drk-baden.de"/>
-    <hyperlink ref="F103" r:id="rId50"/>
-    <hyperlink ref="G103" r:id="rId51" display="mailto:sekretariat.giessen@drk-hessen.de"/>
-    <hyperlink ref="F104" r:id="rId52" display="http://www.kv-trier-saarburg.drk.de/"/>
-    <hyperlink ref="G104" r:id="rId53" display="mailto:info@kv-trier-saarburg.drk.de"/>
+    <hyperlink ref="G139" r:id="rId37"/>
+    <hyperlink ref="F139" r:id="rId38" display="mailto:office@berlin.msf.org"/>
+    <hyperlink ref="G140" r:id="rId39"/>
+    <hyperlink ref="F141" r:id="rId40" display="mailto:info@drk-westfalen.de"/>
+    <hyperlink ref="F142" r:id="rId41"/>
+    <hyperlink ref="G142" r:id="rId42"/>
+    <hyperlink ref="G141" r:id="rId43"/>
+    <hyperlink ref="G143" r:id="rId44"/>
+    <hyperlink ref="F143" r:id="rId45" display="mailto:info@drk-lv-brandenburg.de"/>
+    <hyperlink ref="G145" r:id="rId46" display="http://www.drk-berlin.de/"/>
+    <hyperlink ref="F145" r:id="rId47" display="mailto:drk@drk-berlin.de"/>
+    <hyperlink ref="F146" r:id="rId48" display="http://www.drk-baden.de/"/>
+    <hyperlink ref="G146" r:id="rId49" display="mailto:pressestelle@drk-baden.de"/>
+    <hyperlink ref="F147" r:id="rId50"/>
+    <hyperlink ref="G147" r:id="rId51" display="mailto:sekretariat.giessen@drk-hessen.de"/>
+    <hyperlink ref="F148" r:id="rId52" display="http://www.kv-trier-saarburg.drk.de/"/>
+    <hyperlink ref="G148" r:id="rId53" display="mailto:info@kv-trier-saarburg.drk.de"/>
     <hyperlink ref="F3" r:id="rId54"/>
     <hyperlink ref="F6" r:id="rId55"/>
     <hyperlink ref="F9" r:id="rId56"/>
@@ -5797,8 +8233,8 @@
     <hyperlink ref="F31" r:id="rId59"/>
     <hyperlink ref="F33" r:id="rId60"/>
     <hyperlink ref="F40" r:id="rId61"/>
-    <hyperlink ref="G100" r:id="rId62" display="http://www.drk-berlin.de/"/>
-    <hyperlink ref="F100" r:id="rId63" display="mailto:drk@drk-berlin.de"/>
+    <hyperlink ref="G144" r:id="rId62" display="http://www.drk-berlin.de/"/>
+    <hyperlink ref="F144" r:id="rId63" display="mailto:drk@drk-berlin.de"/>
     <hyperlink ref="G66" r:id="rId64"/>
     <hyperlink ref="G67" r:id="rId65"/>
     <hyperlink ref="F68" r:id="rId66" display="mailto:poststelle@basfi.hamburg.de"/>
@@ -5817,18 +8253,62 @@
     <hyperlink ref="G78" r:id="rId79"/>
     <hyperlink ref="F78" r:id="rId80"/>
     <hyperlink ref="F79" r:id="rId81"/>
+    <hyperlink ref="F80" r:id="rId82" tooltip="E-Mail an Stadt Dortmund - Bürgerdienste schreiben" display="mailto:buergerdienste@stadtdo.de"/>
+    <hyperlink ref="F81" r:id="rId83" tooltip="E-Mail an Stadt Dortmund - Bürgerdienste schreiben" display="mailto:buergerdienste@stadtdo.de"/>
+    <hyperlink ref="F82" r:id="rId84" tooltip="E-Mail an Stadt Dortmund - Bürgerdienste schreiben" display="mailto:buergerdienste@stadtdo.de"/>
+    <hyperlink ref="F83" r:id="rId85" tooltip="E-Mail an Stadt Dortmund - Bürgerdienste schreiben" display="mailto:buergerdienste@stadtdo.de"/>
+    <hyperlink ref="G80" r:id="rId86" tooltip="In neuem Fenster öffnen: http://buergerdienste.dortmund.de" display="http://buergerdienste.dortmund.de/"/>
+    <hyperlink ref="G81" r:id="rId87" tooltip="In neuem Fenster öffnen: http://buergerdienste.dortmund.de" display="http://buergerdienste.dortmund.de/"/>
+    <hyperlink ref="G82" r:id="rId88" tooltip="In neuem Fenster öffnen: http://buergerdienste.dortmund.de" display="http://buergerdienste.dortmund.de/"/>
+    <hyperlink ref="G83" r:id="rId89" tooltip="In neuem Fenster öffnen: http://buergerdienste.dortmund.de" display="http://buergerdienste.dortmund.de/"/>
+    <hyperlink ref="F89" r:id="rId90" display="mailto:zentralemeldebehoerde@stadtamt.bremen.de"/>
+    <hyperlink ref="F106" r:id="rId91" display="mailto:stadtbuero@giessen.de"/>
+    <hyperlink ref="F105" r:id="rId92" display="mailto:stadtbuero@giessen.de"/>
+    <hyperlink ref="F108" r:id="rId93" display="mailto:stadtbuero@giessen.de"/>
+    <hyperlink ref="F110" r:id="rId94" display="mailto:stadtbuero@giessen.de"/>
+    <hyperlink ref="F107" r:id="rId95" display="mailto:stadtbuero@giessen.de"/>
+    <hyperlink ref="F109" r:id="rId96" display="mailto:stadtbuero@giessen.de"/>
+    <hyperlink ref="F149" r:id="rId97" display="javascript:linkTo_UnCryptMailto('kygjrm8ucjamkcYzcpjglcp+rydcj,bc');"/>
+    <hyperlink ref="G149" r:id="rId98"/>
+    <hyperlink ref="G151" r:id="rId99" tooltip="Münchner Tafel e.V." display="http://www.muenchner-tafel.de/"/>
+    <hyperlink ref="F151" r:id="rId100" display="javascript:linkTo_UnCryptMailto('kygjrm8gldmYksclaflcp+rydcj,bc');"/>
+    <hyperlink ref="F150" r:id="rId101" display="javascript:linkTo_UnCryptMailto('kygjrm8gldmYfykzspecp+rydcj,bc');"/>
+    <hyperlink ref="G150" r:id="rId102" tooltip="Hamburger Tafel e.V." display="http://www.hamburger-tafel.de/"/>
+    <hyperlink ref="F154" r:id="rId103" display="javascript:linkTo_UnCryptMailto('kygjrm8kygjYqrsrreyprcp+rydcj,bc');"/>
+    <hyperlink ref="G154" r:id="rId104" tooltip="Bad Cannstatter Tafel" display="http://www.schwaebische-tafel-stuttgart.de/"/>
+    <hyperlink ref="F162" r:id="rId105" display="javascript:linkTo_UnCryptMailto('kygjrm8egcqqclcp,rydcjYbgyimlgc+egcqqcl,bc');"/>
+    <hyperlink ref="G162" r:id="rId106" tooltip="Gießener Tafel" display="http://www.giessener-tafel.de/"/>
+    <hyperlink ref="F161" r:id="rId107" display="javascript:linkTo_UnCryptMailto('kygjrm8gldmYbpcqblcp+rydcj,bc');"/>
+    <hyperlink ref="G161" r:id="rId108" tooltip="Dresdner Tafel e.V." display="http://www.dresdner-tafel.de/"/>
+    <hyperlink ref="F160" r:id="rId109" display="javascript:linkTo_UnCryptMailto('kygjrm8f,lcskycpicpYqid+rpgcp,bc');"/>
+    <hyperlink ref="G160" r:id="rId110" tooltip="Trierer Tafel" display="http://www.skf-trier.de/"/>
+    <hyperlink ref="F159" r:id="rId111" display="javascript:linkTo_UnCryptMailto('kygjrm8imlryirYjcgnxgecp+rydcj,bc');"/>
+    <hyperlink ref="G159" r:id="rId112" tooltip="Leipziger Tafel e.V." display="http://www.leipziger-tafel.de/"/>
+    <hyperlink ref="F158" r:id="rId113" display="javascript:linkTo_UnCryptMailto('kygjrm8zpckclrydcjYlmpb+amk,lcr');"/>
+    <hyperlink ref="G158" r:id="rId114" tooltip="Bremer Tafel e.V." display="http://www.bremertafel.de/"/>
+    <hyperlink ref="F157" r:id="rId115" display="javascript:linkTo_UnCryptMailto('kygjrm8cqqclcp_rydcjYekv,bc');"/>
+    <hyperlink ref="G157" r:id="rId116" tooltip="Essener Tafel e. V." display="http://www.essener-tafel.de/"/>
+    <hyperlink ref="F156" r:id="rId117" display="javascript:linkTo_UnCryptMailto('kygjrm8gldmYbmprkslbcp+rydcj,bc');"/>
+    <hyperlink ref="G156" r:id="rId118" tooltip="Dortmunder Tafel e. V." display="http://www.dortmunder-tafel.de/"/>
+    <hyperlink ref="F155" r:id="rId119" display="javascript:linkTo_UnCryptMailto('kygjrm8gldmYbscqqcjbmpdcp+rydcj,bc');"/>
+    <hyperlink ref="G155" r:id="rId120" tooltip="Düsseldorfer Tafel e.V." display="http://www.duesseldorfer-tafel.de/"/>
+    <hyperlink ref="F153" r:id="rId121" display="javascript:linkTo_UnCryptMailto('kygjrm8dpylidsprcprydcjYr+mljglc,bc');"/>
+    <hyperlink ref="G153" r:id="rId122" tooltip="Frankfurter Tafel e.V." display="http://www.frankfurter-tafel.de/"/>
+    <hyperlink ref="F152" r:id="rId123" display="javascript:linkTo_UnCryptMailto('kygjrm8gldmYimcjlcp+rydcj,bc');"/>
+    <hyperlink ref="G152" r:id="rId124" tooltip="Kölner Tafel e.V." display="http://www.koelner-tafel.de/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId125"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5840,15 +8320,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -5856,7 +8336,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="14">
         <v>2</v>
@@ -5864,7 +8344,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="14">
         <v>3</v>
@@ -5872,7 +8352,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B5" s="14">
         <v>4</v>
@@ -5880,7 +8360,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B6" s="14">
         <v>5</v>
@@ -5888,7 +8368,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B7" s="14">
         <v>6</v>
@@ -5896,7 +8376,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B8" s="14">
         <v>7</v>
@@ -5904,7 +8384,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B9" s="14">
         <v>8</v>
@@ -5912,7 +8392,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B10" s="14">
         <v>9</v>
@@ -5920,7 +8400,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B11" s="14">
         <v>10</v>
@@ -5928,7 +8408,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B12" s="14">
         <v>11</v>
@@ -5936,7 +8416,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B13" s="14">
         <v>12</v>
@@ -5944,10 +8424,26 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B14" s="14">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="B16" s="14">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -6079,7 +8575,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6199,7 +8695,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6355,7 +8851,7 @@
         <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6371,7 +8867,7 @@
         <v>248</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
         <v>249</v>
@@ -6379,7 +8875,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>254</v>
@@ -6387,82 +8883,82 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>